<commit_message>
sullivan.py is now developed for the specific calibration and demonstrates how to use the modules correctly for a specific calibration.
</commit_message>
<xml_diff>
--- a/InductorSet_final.xlsx
+++ b/InductorSet_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\KJ\PycharmProjects\UniversalBridge3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62E5995C-4563-4D4E-873F-6A555D828C4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172F9EDE-A73B-4E4C-8B04-EFF5E1234A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1215" yWindow="4785" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commentary" sheetId="24" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <definedName name="Uncertainty">#REF!</definedName>
     <definedName name="zeros">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="50"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3266,11 +3266,11 @@
   </sheetPr>
   <dimension ref="A1:AQ23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:W23"/>
+      <selection pane="bottomRight" activeCell="Z1" sqref="Z1:AI23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6035,7 +6035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC1CAAA-3BCF-4A51-B8ED-6F1D21918E0E}">
   <dimension ref="A3:I25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>

</xml_diff>